<commit_message>
updated libraries to fix broken links
</commit_message>
<xml_diff>
--- a/wiki/arm_switcher/BOM.xlsx
+++ b/wiki/arm_switcher/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CB39FE-EA9F-47C0-B601-F908F950C6C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA917B93-625B-4604-A8BF-90A1DF293A2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Model</t>
   </si>
@@ -415,7 +415,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -536,6 +536,9 @@
       <c r="A7" t="s">
         <v>15</v>
       </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
       <c r="C7">
         <v>1</v>
       </c>
@@ -550,6 +553,9 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0.5</v>

</xml_diff>